<commit_message>
actualizacion de reporte de actividades y envio de dias de la familia
</commit_message>
<xml_diff>
--- a/Reporte Actividades/2022/12.dic/19 dic.xlsx
+++ b/Reporte Actividades/2022/12.dic/19 dic.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="60">
   <si>
     <t xml:space="preserve">MA- MEJORAS Y MANTENIMIENTO DE APLICACIONES </t>
   </si>
@@ -208,6 +208,15 @@
   </si>
   <si>
     <t>Adquision de Datos Prueba de operacion rango de operacion completo del motor de 10 a 200 rpm, validacion de funcionamiento, datalogger , y funcionalidad de operacion normal.</t>
+  </si>
+  <si>
+    <t>Liberacion de equipo de frontera, prueba de comunicacion de sensor de fondo, validacion de funcionamiento de motor con el motor de banco encontrados, validacion del PQM valores anormales de potencia activa , y factor de potencia entregado por la red</t>
+  </si>
+  <si>
+    <t>Compensatorio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gestion de Viaje, compensatorio, y dias de la familia </t>
   </si>
 </sst>
 </file>
@@ -2065,8 +2074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AX32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11:R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2083,7 +2092,7 @@
     <col min="11" max="11" width="7.140625" customWidth="1"/>
     <col min="12" max="12" width="7.5703125" customWidth="1"/>
     <col min="13" max="13" width="8.85546875" customWidth="1"/>
-    <col min="14" max="14" width="18.5703125" customWidth="1"/>
+    <col min="14" max="14" width="33.140625" customWidth="1"/>
     <col min="15" max="16" width="11.42578125" customWidth="1"/>
     <col min="17" max="17" width="8.5703125" customWidth="1"/>
     <col min="18" max="18" width="16.5703125" customWidth="1"/>
@@ -2508,25 +2517,15 @@
         <v>46</v>
       </c>
       <c r="N9" s="29"/>
-      <c r="O9" s="7">
-        <v>40</v>
-      </c>
-      <c r="P9" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q9" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="R9" s="16"/>
-      <c r="S9" s="7">
-        <v>30</v>
-      </c>
-      <c r="T9" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="U9" s="7" t="s">
-        <v>46</v>
-      </c>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
       <c r="V9" s="7"/>
       <c r="W9" s="7"/>
       <c r="X9" s="7"/>
@@ -2569,7 +2568,7 @@
       <c r="AC10" s="7"/>
       <c r="AD10" s="7"/>
     </row>
-    <row r="11" spans="1:30" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>2</v>
       </c>
@@ -2601,9 +2600,11 @@
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
-      <c r="N11" s="33"/>
+      <c r="N11" s="33" t="s">
+        <v>57</v>
+      </c>
       <c r="O11" s="7">
-        <v>30</v>
+        <v>95</v>
       </c>
       <c r="P11" s="7" t="s">
         <v>45</v>
@@ -2612,15 +2613,9 @@
         <v>46</v>
       </c>
       <c r="R11" s="16"/>
-      <c r="S11" s="7">
-        <v>25</v>
-      </c>
-      <c r="T11" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="U11" s="7" t="s">
-        <v>46</v>
-      </c>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
       <c r="V11" s="7"/>
       <c r="W11" s="7"/>
       <c r="X11" s="7"/>
@@ -2684,15 +2679,9 @@
       <c r="P13" s="8"/>
       <c r="Q13" s="8"/>
       <c r="R13" s="29"/>
-      <c r="S13" s="8">
-        <v>45</v>
-      </c>
-      <c r="T13" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="U13" s="7" t="s">
-        <v>46</v>
-      </c>
+      <c r="S13" s="8"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
       <c r="V13" s="8"/>
       <c r="W13" s="8"/>
       <c r="X13" s="8"/>
@@ -2833,9 +2822,11 @@
       <c r="M17" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="N17" s="7"/>
+      <c r="N17" s="16" t="s">
+        <v>59</v>
+      </c>
       <c r="O17" s="7">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="P17" s="7" t="s">
         <v>45</v>
@@ -2871,7 +2862,7 @@
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
       <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
+      <c r="N18" s="16"/>
       <c r="O18" s="7"/>
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
@@ -3635,6 +3626,7 @@
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="G9:G10"/>
+    <mergeCell ref="N9:N10"/>
     <mergeCell ref="Q17:Q18"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="U13:U14"/>
@@ -3683,8 +3675,6 @@
     <mergeCell ref="AC7:AC8"/>
     <mergeCell ref="Q7:Q8"/>
     <mergeCell ref="P17:P18"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="R9:R10"/>
     <mergeCell ref="O13:O14"/>
     <mergeCell ref="O15:O16"/>
     <mergeCell ref="S9:S10"/>
@@ -3743,6 +3733,7 @@
     <mergeCell ref="S7:S8"/>
     <mergeCell ref="Y7:Y8"/>
     <mergeCell ref="V9:V10"/>
+    <mergeCell ref="R9:R10"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="B7:B8"/>

</xml_diff>